<commit_message>
added evaluation file for content, wanna add yours for the XML? Replaced comments llama with the correct file
</commit_message>
<xml_diff>
--- a/chapter1_ZA-content/results/llama_herd/comments_llama.xlsx
+++ b/chapter1_ZA-content/results/llama_herd/comments_llama.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lizzi\Downloads\python_projects\test_objects\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C6AA92ED-C583-4612-9DBA-5E3D961F6316}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BBA6A3B5-D998-4229-B531-F1F40B6534E7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-90" yWindow="0" windowWidth="12180" windowHeight="15370" activeTab="1" xr2:uid="{DB4E80FD-8B0C-4E09-A1FB-55FCDD1AF76F}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="24220" windowHeight="15500" activeTab="1" xr2:uid="{DB4E80FD-8B0C-4E09-A1FB-55FCDD1AF76F}"/>
   </bookViews>
   <sheets>
     <sheet name="13.12" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="309" uniqueCount="69">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="290" uniqueCount="59">
   <si>
     <t xml:space="preserve">File </t>
   </si>
@@ -147,33 +147,6 @@
     <t>test_27</t>
   </si>
   <si>
-    <t>test_28</t>
-  </si>
-  <si>
-    <t>test_29</t>
-  </si>
-  <si>
-    <t>test_30</t>
-  </si>
-  <si>
-    <t>test_31</t>
-  </si>
-  <si>
-    <t>test_32</t>
-  </si>
-  <si>
-    <t>test_33</t>
-  </si>
-  <si>
-    <t>test_34</t>
-  </si>
-  <si>
-    <t>test_35</t>
-  </si>
-  <si>
-    <t>llama 3.1 8B instruct</t>
-  </si>
-  <si>
     <t>Answer: Be a helpful assistant</t>
   </si>
   <si>
@@ -189,9 +162,6 @@
     <t>Given: {example_txt} with the goal: {example_xml}, format this: {chunk} into the same xml format. Format all of the text. Give only the formated text.</t>
   </si>
   <si>
-    <t xml:space="preserve">llama 3 3B </t>
-  </si>
-  <si>
     <t>If given raw text: {example_txt} with the end goal: {example_xml}, adapt this: {chunk} into the same xml format.</t>
   </si>
   <si>
@@ -204,15 +174,9 @@
     <t>Files</t>
   </si>
   <si>
-    <t>llama 3 1B</t>
-  </si>
-  <si>
     <t xml:space="preserve">Answer: Be a helpful assistant. </t>
   </si>
   <si>
-    <t>llama 3 3B</t>
-  </si>
-  <si>
     <t xml:space="preserve">llama 3 8B </t>
   </si>
   <si>
@@ -237,13 +201,19 @@
     <t>llama 3.2 3B</t>
   </si>
   <si>
-    <t>input: {example_txt} output: {example_xml}. Observe the example input and output. Format {chunk} into the same xml format. Format all of the text. Give only the formated text</t>
-  </si>
-  <si>
     <t>Nan</t>
   </si>
   <si>
     <t>The CHIEF WHIP OF THE MAJORITY PARTY: Thank you very much, House Chair. As indicated on the Order Paper we shall proceed.</t>
+  </si>
+  <si>
+    <t>llama 3 8B instruct</t>
+  </si>
+  <si>
+    <t xml:space="preserve">llama 3.2 3B </t>
+  </si>
+  <si>
+    <t>llama 3.2 1B</t>
   </si>
 </sst>
 </file>
@@ -626,19 +596,20 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0DA51448-A8CB-44AC-8E4D-0C35693C4BE5}">
   <dimension ref="A1:J25"/>
   <sheetViews>
-    <sheetView topLeftCell="A11" workbookViewId="0">
-      <selection activeCell="I28" sqref="I28"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F5" sqref="F5:F25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
+    <col min="2" max="2" width="18.08984375" customWidth="1"/>
     <col min="9" max="9" width="43.6328125" style="1" customWidth="1"/>
     <col min="10" max="10" width="17.26953125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
-        <v>54</v>
+        <v>44</v>
       </c>
       <c r="B1" t="s">
         <v>1</v>
@@ -665,7 +636,7 @@
         <v>6</v>
       </c>
       <c r="J1" t="s">
-        <v>63</v>
+        <v>51</v>
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.35">
@@ -673,13 +644,13 @@
         <v>9</v>
       </c>
       <c r="B2" t="s">
-        <v>50</v>
+        <v>57</v>
       </c>
       <c r="C2" t="s">
-        <v>67</v>
+        <v>54</v>
       </c>
       <c r="D2" t="s">
-        <v>52</v>
+        <v>42</v>
       </c>
       <c r="E2">
         <v>4</v>
@@ -688,13 +659,13 @@
         <v>1000</v>
       </c>
       <c r="G2" t="s">
-        <v>62</v>
+        <v>50</v>
       </c>
       <c r="H2" t="s">
-        <v>68</v>
+        <v>55</v>
       </c>
       <c r="I2" t="s">
-        <v>51</v>
+        <v>41</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.35">
@@ -702,13 +673,13 @@
         <v>10</v>
       </c>
       <c r="B3" t="s">
-        <v>50</v>
+        <v>57</v>
       </c>
       <c r="C3" t="s">
-        <v>67</v>
+        <v>54</v>
       </c>
       <c r="D3" t="s">
-        <v>52</v>
+        <v>42</v>
       </c>
       <c r="E3">
         <v>4</v>
@@ -717,13 +688,13 @@
         <v>1000</v>
       </c>
       <c r="G3" t="s">
-        <v>62</v>
+        <v>50</v>
       </c>
       <c r="H3" t="s">
-        <v>68</v>
+        <v>55</v>
       </c>
       <c r="I3" t="s">
-        <v>53</v>
+        <v>43</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.35">
@@ -731,13 +702,13 @@
         <v>11</v>
       </c>
       <c r="B4" t="s">
-        <v>50</v>
+        <v>57</v>
       </c>
       <c r="C4" t="s">
-        <v>67</v>
+        <v>54</v>
       </c>
       <c r="D4" t="s">
-        <v>52</v>
+        <v>42</v>
       </c>
       <c r="E4">
         <v>4</v>
@@ -746,13 +717,13 @@
         <v>1000</v>
       </c>
       <c r="G4" t="s">
-        <v>62</v>
+        <v>50</v>
       </c>
       <c r="H4" t="s">
-        <v>68</v>
+        <v>55</v>
       </c>
       <c r="I4" t="s">
-        <v>53</v>
+        <v>43</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.35">
@@ -760,13 +731,13 @@
         <v>12</v>
       </c>
       <c r="B5" t="s">
-        <v>50</v>
+        <v>57</v>
       </c>
       <c r="C5" t="s">
-        <v>67</v>
+        <v>54</v>
       </c>
       <c r="D5" t="s">
-        <v>52</v>
+        <v>42</v>
       </c>
       <c r="E5">
         <v>4</v>
@@ -775,13 +746,13 @@
         <v>1000</v>
       </c>
       <c r="G5" t="s">
-        <v>62</v>
+        <v>50</v>
       </c>
       <c r="H5" t="s">
-        <v>68</v>
+        <v>55</v>
       </c>
       <c r="I5" t="s">
-        <v>53</v>
+        <v>43</v>
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.35">
@@ -789,25 +760,28 @@
         <v>13</v>
       </c>
       <c r="B6" t="s">
-        <v>55</v>
+        <v>58</v>
       </c>
       <c r="C6" t="s">
-        <v>67</v>
+        <v>54</v>
       </c>
       <c r="D6" t="s">
-        <v>52</v>
+        <v>42</v>
       </c>
       <c r="E6">
         <v>4</v>
       </c>
+      <c r="F6">
+        <v>1000</v>
+      </c>
       <c r="G6" t="s">
-        <v>62</v>
+        <v>50</v>
       </c>
       <c r="H6" t="s">
-        <v>68</v>
+        <v>55</v>
       </c>
       <c r="I6" t="s">
-        <v>53</v>
+        <v>43</v>
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.35">
@@ -815,25 +789,28 @@
         <v>14</v>
       </c>
       <c r="B7" t="s">
-        <v>55</v>
+        <v>58</v>
       </c>
       <c r="C7" t="s">
-        <v>67</v>
+        <v>54</v>
       </c>
       <c r="D7" t="s">
-        <v>52</v>
+        <v>42</v>
       </c>
       <c r="E7">
         <v>4</v>
       </c>
+      <c r="F7">
+        <v>1000</v>
+      </c>
       <c r="G7" t="s">
-        <v>62</v>
+        <v>50</v>
       </c>
       <c r="H7" t="s">
-        <v>68</v>
+        <v>55</v>
       </c>
       <c r="I7" t="s">
-        <v>53</v>
+        <v>43</v>
       </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.35">
@@ -841,25 +818,28 @@
         <v>15</v>
       </c>
       <c r="B8" t="s">
-        <v>55</v>
+        <v>58</v>
       </c>
       <c r="C8" t="s">
-        <v>67</v>
+        <v>54</v>
       </c>
       <c r="D8" t="s">
-        <v>56</v>
+        <v>45</v>
       </c>
       <c r="E8">
         <v>4</v>
       </c>
+      <c r="F8">
+        <v>1000</v>
+      </c>
       <c r="G8" t="s">
-        <v>62</v>
+        <v>50</v>
       </c>
       <c r="H8" t="s">
-        <v>68</v>
+        <v>55</v>
       </c>
       <c r="I8" t="s">
-        <v>53</v>
+        <v>43</v>
       </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.35">
@@ -867,25 +847,28 @@
         <v>16</v>
       </c>
       <c r="B9" t="s">
-        <v>55</v>
+        <v>58</v>
       </c>
       <c r="C9" t="s">
-        <v>67</v>
+        <v>54</v>
       </c>
       <c r="D9" t="s">
-        <v>56</v>
+        <v>45</v>
       </c>
       <c r="E9">
         <v>4</v>
       </c>
+      <c r="F9">
+        <v>1000</v>
+      </c>
       <c r="G9" t="s">
-        <v>62</v>
+        <v>50</v>
       </c>
       <c r="H9" t="s">
-        <v>68</v>
+        <v>55</v>
       </c>
       <c r="I9" t="s">
-        <v>53</v>
+        <v>43</v>
       </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.35">
@@ -893,25 +876,28 @@
         <v>17</v>
       </c>
       <c r="B10" t="s">
-        <v>55</v>
+        <v>58</v>
       </c>
       <c r="C10" t="s">
-        <v>67</v>
+        <v>54</v>
       </c>
       <c r="D10" t="s">
-        <v>56</v>
+        <v>45</v>
       </c>
       <c r="E10">
         <v>4</v>
       </c>
+      <c r="F10">
+        <v>1000</v>
+      </c>
       <c r="G10" t="s">
-        <v>62</v>
+        <v>50</v>
       </c>
       <c r="H10" t="s">
-        <v>68</v>
+        <v>55</v>
       </c>
       <c r="I10" t="s">
-        <v>53</v>
+        <v>43</v>
       </c>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.35">
@@ -919,25 +905,28 @@
         <v>18</v>
       </c>
       <c r="B11" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="C11" t="s">
-        <v>67</v>
+        <v>54</v>
       </c>
       <c r="D11" t="s">
-        <v>56</v>
+        <v>45</v>
       </c>
       <c r="E11">
         <v>4</v>
       </c>
+      <c r="F11">
+        <v>1000</v>
+      </c>
       <c r="G11" t="s">
-        <v>62</v>
+        <v>50</v>
       </c>
       <c r="H11" t="s">
-        <v>68</v>
+        <v>55</v>
       </c>
       <c r="I11" t="s">
-        <v>53</v>
+        <v>43</v>
       </c>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.35">
@@ -945,25 +934,28 @@
         <v>19</v>
       </c>
       <c r="B12" t="s">
-        <v>50</v>
+        <v>53</v>
       </c>
       <c r="C12" t="s">
-        <v>67</v>
+        <v>54</v>
       </c>
       <c r="D12" t="s">
-        <v>56</v>
+        <v>45</v>
       </c>
       <c r="E12">
         <v>4</v>
       </c>
+      <c r="F12">
+        <v>1000</v>
+      </c>
       <c r="G12" t="s">
-        <v>62</v>
+        <v>50</v>
       </c>
       <c r="H12" t="s">
-        <v>68</v>
+        <v>55</v>
       </c>
       <c r="I12" t="s">
-        <v>53</v>
+        <v>43</v>
       </c>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.35">
@@ -971,25 +963,28 @@
         <v>20</v>
       </c>
       <c r="B13" t="s">
-        <v>50</v>
+        <v>53</v>
       </c>
       <c r="C13" t="s">
-        <v>67</v>
+        <v>54</v>
       </c>
       <c r="D13" t="s">
-        <v>56</v>
+        <v>45</v>
       </c>
       <c r="E13">
         <v>4</v>
       </c>
+      <c r="F13">
+        <v>1000</v>
+      </c>
       <c r="G13" t="s">
-        <v>62</v>
+        <v>50</v>
       </c>
       <c r="H13" t="s">
-        <v>68</v>
+        <v>55</v>
       </c>
       <c r="I13" t="s">
-        <v>53</v>
+        <v>43</v>
       </c>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.35">
@@ -997,25 +992,28 @@
         <v>24</v>
       </c>
       <c r="B14" t="s">
-        <v>58</v>
+        <v>46</v>
       </c>
       <c r="C14" t="s">
-        <v>67</v>
+        <v>54</v>
       </c>
       <c r="D14" t="s">
-        <v>45</v>
+        <v>36</v>
       </c>
       <c r="E14">
         <v>4</v>
       </c>
+      <c r="F14">
+        <v>1000</v>
+      </c>
       <c r="G14" t="s">
-        <v>62</v>
+        <v>50</v>
       </c>
       <c r="H14" t="s">
-        <v>68</v>
+        <v>55</v>
       </c>
       <c r="I14" t="s">
-        <v>59</v>
+        <v>47</v>
       </c>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.35">
@@ -1023,25 +1021,28 @@
         <v>25</v>
       </c>
       <c r="B15" t="s">
-        <v>58</v>
+        <v>46</v>
       </c>
       <c r="C15" t="s">
-        <v>67</v>
+        <v>54</v>
       </c>
       <c r="D15" t="s">
-        <v>45</v>
+        <v>36</v>
       </c>
       <c r="E15">
         <v>4</v>
       </c>
+      <c r="F15">
+        <v>1000</v>
+      </c>
       <c r="G15" t="s">
-        <v>62</v>
+        <v>50</v>
       </c>
       <c r="H15" t="s">
-        <v>68</v>
+        <v>55</v>
       </c>
       <c r="I15" t="s">
-        <v>59</v>
+        <v>47</v>
       </c>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.35">
@@ -1049,25 +1050,28 @@
         <v>26</v>
       </c>
       <c r="B16" t="s">
-        <v>58</v>
+        <v>46</v>
       </c>
       <c r="C16" t="s">
-        <v>67</v>
+        <v>54</v>
       </c>
       <c r="D16" t="s">
-        <v>45</v>
+        <v>36</v>
       </c>
       <c r="E16">
         <v>4</v>
       </c>
+      <c r="F16">
+        <v>1000</v>
+      </c>
       <c r="G16" t="s">
-        <v>62</v>
+        <v>50</v>
       </c>
       <c r="H16" t="s">
-        <v>68</v>
+        <v>55</v>
       </c>
       <c r="I16" t="s">
-        <v>59</v>
+        <v>47</v>
       </c>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.35">
@@ -1075,25 +1079,28 @@
         <v>27</v>
       </c>
       <c r="B17" t="s">
-        <v>58</v>
+        <v>46</v>
       </c>
       <c r="C17" t="s">
-        <v>67</v>
+        <v>54</v>
       </c>
       <c r="D17" t="s">
-        <v>45</v>
+        <v>36</v>
       </c>
       <c r="E17">
         <v>4</v>
       </c>
+      <c r="F17">
+        <v>1000</v>
+      </c>
       <c r="G17" t="s">
-        <v>62</v>
+        <v>50</v>
       </c>
       <c r="H17" t="s">
-        <v>68</v>
+        <v>55</v>
       </c>
       <c r="I17" t="s">
-        <v>60</v>
+        <v>48</v>
       </c>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.35">
@@ -1101,25 +1108,28 @@
         <v>28</v>
       </c>
       <c r="B18" t="s">
-        <v>58</v>
+        <v>46</v>
       </c>
       <c r="C18" t="s">
-        <v>67</v>
+        <v>54</v>
       </c>
       <c r="D18" t="s">
-        <v>45</v>
+        <v>36</v>
       </c>
       <c r="E18">
         <v>4</v>
       </c>
+      <c r="F18">
+        <v>1000</v>
+      </c>
       <c r="G18" t="s">
-        <v>62</v>
+        <v>50</v>
       </c>
       <c r="H18" t="s">
-        <v>68</v>
+        <v>55</v>
       </c>
       <c r="I18" t="s">
-        <v>60</v>
+        <v>48</v>
       </c>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.35">
@@ -1127,25 +1137,28 @@
         <v>29</v>
       </c>
       <c r="B19" t="s">
-        <v>58</v>
+        <v>46</v>
       </c>
       <c r="C19" t="s">
-        <v>67</v>
+        <v>54</v>
       </c>
       <c r="D19" t="s">
-        <v>45</v>
+        <v>36</v>
       </c>
       <c r="E19">
         <v>4</v>
       </c>
+      <c r="F19">
+        <v>1000</v>
+      </c>
       <c r="G19" t="s">
-        <v>62</v>
+        <v>50</v>
       </c>
       <c r="H19" t="s">
-        <v>68</v>
+        <v>55</v>
       </c>
       <c r="I19" t="s">
-        <v>60</v>
+        <v>48</v>
       </c>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.35">
@@ -1153,25 +1166,28 @@
         <v>30</v>
       </c>
       <c r="B20" t="s">
-        <v>58</v>
+        <v>46</v>
       </c>
       <c r="C20" t="s">
-        <v>67</v>
+        <v>54</v>
       </c>
       <c r="D20" t="s">
-        <v>45</v>
+        <v>36</v>
       </c>
       <c r="E20">
         <v>4</v>
       </c>
+      <c r="F20">
+        <v>1000</v>
+      </c>
       <c r="G20" t="s">
-        <v>62</v>
+        <v>50</v>
       </c>
       <c r="H20" t="s">
-        <v>68</v>
+        <v>55</v>
       </c>
       <c r="I20" t="s">
-        <v>61</v>
+        <v>49</v>
       </c>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.35">
@@ -1179,25 +1195,28 @@
         <v>31</v>
       </c>
       <c r="B21" t="s">
-        <v>58</v>
+        <v>46</v>
       </c>
       <c r="C21" t="s">
-        <v>67</v>
+        <v>54</v>
       </c>
       <c r="D21" t="s">
-        <v>45</v>
+        <v>36</v>
       </c>
       <c r="E21">
         <v>4</v>
       </c>
+      <c r="F21">
+        <v>1000</v>
+      </c>
       <c r="G21" t="s">
-        <v>62</v>
+        <v>50</v>
       </c>
       <c r="H21" t="s">
-        <v>68</v>
+        <v>55</v>
       </c>
       <c r="I21" t="s">
-        <v>61</v>
+        <v>49</v>
       </c>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.35">
@@ -1205,25 +1224,28 @@
         <v>32</v>
       </c>
       <c r="B22" t="s">
-        <v>58</v>
+        <v>46</v>
       </c>
       <c r="C22" t="s">
-        <v>67</v>
+        <v>54</v>
       </c>
       <c r="D22" t="s">
-        <v>45</v>
+        <v>36</v>
       </c>
       <c r="E22">
         <v>4</v>
       </c>
+      <c r="F22">
+        <v>1000</v>
+      </c>
       <c r="G22" t="s">
-        <v>62</v>
+        <v>50</v>
       </c>
       <c r="H22" t="s">
-        <v>68</v>
+        <v>55</v>
       </c>
       <c r="I22" t="s">
-        <v>61</v>
+        <v>49</v>
       </c>
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.35">
@@ -1231,25 +1253,28 @@
         <v>33</v>
       </c>
       <c r="B23" t="s">
-        <v>58</v>
+        <v>46</v>
       </c>
       <c r="C23" t="s">
-        <v>67</v>
+        <v>54</v>
       </c>
       <c r="D23" t="s">
-        <v>45</v>
+        <v>36</v>
       </c>
       <c r="E23">
         <v>4</v>
       </c>
+      <c r="F23">
+        <v>1000</v>
+      </c>
       <c r="G23" t="s">
-        <v>62</v>
+        <v>50</v>
       </c>
       <c r="H23" t="s">
-        <v>68</v>
+        <v>55</v>
       </c>
       <c r="I23" t="s">
-        <v>61</v>
+        <v>49</v>
       </c>
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.35">
@@ -1257,25 +1282,28 @@
         <v>34</v>
       </c>
       <c r="B24" t="s">
-        <v>58</v>
+        <v>46</v>
       </c>
       <c r="C24" t="s">
-        <v>67</v>
+        <v>54</v>
       </c>
       <c r="D24" t="s">
-        <v>45</v>
+        <v>36</v>
       </c>
       <c r="E24">
         <v>4</v>
       </c>
+      <c r="F24">
+        <v>1000</v>
+      </c>
       <c r="G24" t="s">
-        <v>62</v>
+        <v>50</v>
       </c>
       <c r="H24" t="s">
-        <v>68</v>
+        <v>55</v>
       </c>
       <c r="I24" t="s">
-        <v>61</v>
+        <v>49</v>
       </c>
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.35">
@@ -1283,25 +1311,28 @@
         <v>35</v>
       </c>
       <c r="B25" t="s">
-        <v>58</v>
+        <v>46</v>
       </c>
       <c r="C25" t="s">
-        <v>67</v>
+        <v>54</v>
       </c>
       <c r="D25" t="s">
-        <v>45</v>
+        <v>36</v>
       </c>
       <c r="E25">
         <v>4</v>
       </c>
+      <c r="F25">
+        <v>1000</v>
+      </c>
       <c r="G25" t="s">
-        <v>62</v>
+        <v>50</v>
       </c>
       <c r="H25" t="s">
-        <v>68</v>
+        <v>55</v>
       </c>
       <c r="I25" t="s">
-        <v>61</v>
+        <v>49</v>
       </c>
     </row>
   </sheetData>
@@ -1317,13 +1348,16 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A7B30784-A0CE-43DD-A639-9259E6DC8F09}">
-  <dimension ref="A1:J36"/>
+  <dimension ref="A1:J19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G2" sqref="G2"/>
+      <selection activeCell="A20" sqref="A20:XFD20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="2" max="2" width="20.26953125" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
@@ -1354,7 +1388,7 @@
         <v>6</v>
       </c>
       <c r="J1" t="s">
-        <v>64</v>
+        <v>52</v>
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.35">
@@ -1362,13 +1396,13 @@
         <v>9</v>
       </c>
       <c r="B2" t="s">
-        <v>44</v>
+        <v>56</v>
       </c>
       <c r="C2">
         <v>0.1</v>
       </c>
       <c r="D2" t="s">
-        <v>45</v>
+        <v>36</v>
       </c>
       <c r="E2">
         <v>4</v>
@@ -1377,13 +1411,13 @@
         <v>1000</v>
       </c>
       <c r="G2" t="s">
-        <v>46</v>
+        <v>37</v>
       </c>
       <c r="H2" t="s">
-        <v>47</v>
+        <v>38</v>
       </c>
       <c r="I2" t="s">
-        <v>48</v>
+        <v>39</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.35">
@@ -1391,13 +1425,13 @@
         <v>10</v>
       </c>
       <c r="B3" t="s">
-        <v>44</v>
+        <v>56</v>
       </c>
       <c r="C3">
         <v>0.1</v>
       </c>
       <c r="D3" t="s">
-        <v>45</v>
+        <v>36</v>
       </c>
       <c r="E3">
         <v>4</v>
@@ -1406,13 +1440,13 @@
         <v>1000</v>
       </c>
       <c r="G3" t="s">
-        <v>46</v>
+        <v>37</v>
       </c>
       <c r="H3" t="s">
-        <v>47</v>
+        <v>38</v>
       </c>
       <c r="I3" t="s">
-        <v>48</v>
+        <v>39</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.35">
@@ -1420,13 +1454,13 @@
         <v>11</v>
       </c>
       <c r="B4" t="s">
-        <v>44</v>
+        <v>56</v>
       </c>
       <c r="C4">
         <v>0.1</v>
       </c>
       <c r="D4" t="s">
-        <v>45</v>
+        <v>36</v>
       </c>
       <c r="E4">
         <v>4</v>
@@ -1435,13 +1469,13 @@
         <v>1000</v>
       </c>
       <c r="G4" t="s">
-        <v>46</v>
+        <v>37</v>
       </c>
       <c r="H4" t="s">
-        <v>47</v>
+        <v>38</v>
       </c>
       <c r="I4" t="s">
-        <v>48</v>
+        <v>39</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.35">
@@ -1449,13 +1483,13 @@
         <v>12</v>
       </c>
       <c r="B5" t="s">
-        <v>44</v>
+        <v>56</v>
       </c>
       <c r="C5">
         <v>0.1</v>
       </c>
       <c r="D5" t="s">
-        <v>45</v>
+        <v>36</v>
       </c>
       <c r="E5">
         <v>4</v>
@@ -1464,13 +1498,13 @@
         <v>1000</v>
       </c>
       <c r="G5" t="s">
-        <v>46</v>
+        <v>37</v>
       </c>
       <c r="H5" t="s">
-        <v>47</v>
+        <v>38</v>
       </c>
       <c r="I5" t="s">
-        <v>49</v>
+        <v>40</v>
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.35">
@@ -1478,13 +1512,13 @@
         <v>13</v>
       </c>
       <c r="B6" t="s">
-        <v>44</v>
+        <v>56</v>
       </c>
       <c r="C6">
         <v>0.1</v>
       </c>
       <c r="D6" t="s">
-        <v>45</v>
+        <v>36</v>
       </c>
       <c r="E6">
         <v>4</v>
@@ -1493,13 +1527,13 @@
         <v>1000</v>
       </c>
       <c r="G6" t="s">
-        <v>46</v>
+        <v>37</v>
       </c>
       <c r="H6" t="s">
-        <v>47</v>
+        <v>38</v>
       </c>
       <c r="I6" t="s">
-        <v>49</v>
+        <v>40</v>
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.35">
@@ -1507,13 +1541,13 @@
         <v>14</v>
       </c>
       <c r="B7" t="s">
-        <v>44</v>
+        <v>56</v>
       </c>
       <c r="C7">
         <v>0.1</v>
       </c>
       <c r="D7" t="s">
-        <v>45</v>
+        <v>36</v>
       </c>
       <c r="E7">
         <v>4</v>
@@ -1522,13 +1556,13 @@
         <v>1000</v>
       </c>
       <c r="G7" t="s">
-        <v>46</v>
+        <v>37</v>
       </c>
       <c r="H7" t="s">
-        <v>47</v>
+        <v>38</v>
       </c>
       <c r="I7" t="s">
-        <v>49</v>
+        <v>40</v>
       </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.35">
@@ -1536,13 +1570,13 @@
         <v>15</v>
       </c>
       <c r="B8" t="s">
-        <v>44</v>
+        <v>56</v>
       </c>
       <c r="C8">
         <v>0.05</v>
       </c>
       <c r="D8" t="s">
-        <v>45</v>
+        <v>36</v>
       </c>
       <c r="E8">
         <v>4</v>
@@ -1551,13 +1585,13 @@
         <v>1000</v>
       </c>
       <c r="G8" t="s">
-        <v>46</v>
+        <v>37</v>
       </c>
       <c r="H8" t="s">
-        <v>47</v>
+        <v>38</v>
       </c>
       <c r="I8" t="s">
-        <v>49</v>
+        <v>40</v>
       </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.35">
@@ -1565,13 +1599,13 @@
         <v>16</v>
       </c>
       <c r="B9" t="s">
-        <v>44</v>
+        <v>56</v>
       </c>
       <c r="C9">
         <v>0.05</v>
       </c>
       <c r="D9" t="s">
-        <v>45</v>
+        <v>36</v>
       </c>
       <c r="E9">
         <v>4</v>
@@ -1580,13 +1614,13 @@
         <v>1000</v>
       </c>
       <c r="G9" t="s">
-        <v>46</v>
+        <v>37</v>
       </c>
       <c r="H9" t="s">
-        <v>47</v>
+        <v>38</v>
       </c>
       <c r="I9" t="s">
-        <v>49</v>
+        <v>40</v>
       </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.35">
@@ -1594,13 +1628,13 @@
         <v>17</v>
       </c>
       <c r="B10" t="s">
-        <v>44</v>
+        <v>56</v>
       </c>
       <c r="C10">
         <v>0.05</v>
       </c>
       <c r="D10" t="s">
-        <v>45</v>
+        <v>36</v>
       </c>
       <c r="E10">
         <v>4</v>
@@ -1609,13 +1643,13 @@
         <v>1000</v>
       </c>
       <c r="G10" t="s">
-        <v>46</v>
+        <v>37</v>
       </c>
       <c r="H10" t="s">
-        <v>47</v>
+        <v>38</v>
       </c>
       <c r="I10" t="s">
-        <v>49</v>
+        <v>40</v>
       </c>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.35">
@@ -1623,13 +1657,13 @@
         <v>18</v>
       </c>
       <c r="B11" t="s">
-        <v>44</v>
+        <v>56</v>
       </c>
       <c r="C11">
         <v>0</v>
       </c>
       <c r="D11" t="s">
-        <v>45</v>
+        <v>36</v>
       </c>
       <c r="E11">
         <v>4</v>
@@ -1638,13 +1672,13 @@
         <v>1000</v>
       </c>
       <c r="G11" t="s">
-        <v>46</v>
+        <v>37</v>
       </c>
       <c r="H11" t="s">
-        <v>47</v>
+        <v>38</v>
       </c>
       <c r="I11" t="s">
-        <v>49</v>
+        <v>40</v>
       </c>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.35">
@@ -1652,13 +1686,13 @@
         <v>19</v>
       </c>
       <c r="B12" t="s">
-        <v>44</v>
+        <v>56</v>
       </c>
       <c r="C12">
         <v>0</v>
       </c>
       <c r="D12" t="s">
-        <v>45</v>
+        <v>36</v>
       </c>
       <c r="E12">
         <v>4</v>
@@ -1667,13 +1701,13 @@
         <v>1000</v>
       </c>
       <c r="G12" t="s">
-        <v>46</v>
+        <v>37</v>
       </c>
       <c r="H12" t="s">
-        <v>47</v>
+        <v>38</v>
       </c>
       <c r="I12" t="s">
-        <v>49</v>
+        <v>40</v>
       </c>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.35">
@@ -1681,13 +1715,13 @@
         <v>20</v>
       </c>
       <c r="B13" t="s">
-        <v>44</v>
+        <v>56</v>
       </c>
       <c r="C13">
         <v>0</v>
       </c>
       <c r="D13" t="s">
-        <v>45</v>
+        <v>36</v>
       </c>
       <c r="E13">
         <v>4</v>
@@ -1696,13 +1730,13 @@
         <v>1000</v>
       </c>
       <c r="G13" t="s">
-        <v>46</v>
+        <v>37</v>
       </c>
       <c r="H13" t="s">
-        <v>47</v>
+        <v>38</v>
       </c>
       <c r="I13" t="s">
-        <v>49</v>
+        <v>40</v>
       </c>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.35">
@@ -1710,13 +1744,13 @@
         <v>21</v>
       </c>
       <c r="B14" t="s">
-        <v>44</v>
+        <v>56</v>
       </c>
       <c r="C14">
         <v>0</v>
       </c>
       <c r="D14" t="s">
-        <v>45</v>
+        <v>36</v>
       </c>
       <c r="E14">
         <v>8</v>
@@ -1725,10 +1759,10 @@
         <v>1000</v>
       </c>
       <c r="G14" t="s">
-        <v>46</v>
+        <v>37</v>
       </c>
       <c r="I14" t="s">
-        <v>49</v>
+        <v>40</v>
       </c>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.35">
@@ -1736,13 +1770,13 @@
         <v>22</v>
       </c>
       <c r="B15" t="s">
-        <v>44</v>
+        <v>56</v>
       </c>
       <c r="C15">
         <v>0</v>
       </c>
       <c r="D15" t="s">
-        <v>45</v>
+        <v>36</v>
       </c>
       <c r="E15">
         <v>8</v>
@@ -1751,10 +1785,10 @@
         <v>1000</v>
       </c>
       <c r="G15" t="s">
-        <v>46</v>
+        <v>37</v>
       </c>
       <c r="I15" t="s">
-        <v>49</v>
+        <v>40</v>
       </c>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.35">
@@ -1762,13 +1796,13 @@
         <v>23</v>
       </c>
       <c r="B16" t="s">
-        <v>44</v>
+        <v>56</v>
       </c>
       <c r="C16">
         <v>0</v>
       </c>
       <c r="D16" t="s">
-        <v>45</v>
+        <v>36</v>
       </c>
       <c r="E16">
         <v>8</v>
@@ -1777,10 +1811,10 @@
         <v>1000</v>
       </c>
       <c r="G16" t="s">
-        <v>46</v>
+        <v>37</v>
       </c>
       <c r="I16" t="s">
-        <v>49</v>
+        <v>40</v>
       </c>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.35">
@@ -1788,13 +1822,13 @@
         <v>24</v>
       </c>
       <c r="B17" t="s">
-        <v>65</v>
+        <v>53</v>
       </c>
       <c r="C17">
         <v>0</v>
       </c>
       <c r="D17" t="s">
-        <v>45</v>
+        <v>36</v>
       </c>
       <c r="E17">
         <v>4</v>
@@ -1803,10 +1837,10 @@
         <v>1000</v>
       </c>
       <c r="G17" t="s">
-        <v>46</v>
+        <v>37</v>
       </c>
       <c r="I17" t="s">
-        <v>49</v>
+        <v>40</v>
       </c>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.35">
@@ -1814,13 +1848,13 @@
         <v>25</v>
       </c>
       <c r="B18" t="s">
-        <v>65</v>
+        <v>53</v>
       </c>
       <c r="C18">
         <v>0</v>
       </c>
       <c r="D18" t="s">
-        <v>45</v>
+        <v>36</v>
       </c>
       <c r="E18">
         <v>4</v>
@@ -1829,10 +1863,10 @@
         <v>1000</v>
       </c>
       <c r="G18" t="s">
-        <v>46</v>
+        <v>37</v>
       </c>
       <c r="I18" t="s">
-        <v>49</v>
+        <v>40</v>
       </c>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.35">
@@ -1840,13 +1874,13 @@
         <v>26</v>
       </c>
       <c r="B19" t="s">
-        <v>65</v>
+        <v>53</v>
       </c>
       <c r="C19">
         <v>0</v>
       </c>
       <c r="D19" t="s">
-        <v>45</v>
+        <v>36</v>
       </c>
       <c r="E19">
         <v>4</v>
@@ -1855,101 +1889,10 @@
         <v>1000</v>
       </c>
       <c r="G19" t="s">
-        <v>46</v>
+        <v>37</v>
       </c>
       <c r="I19" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A20" t="s">
-        <v>27</v>
-      </c>
-      <c r="B20" t="s">
-        <v>44</v>
-      </c>
-      <c r="I20" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A21" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A22" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A23" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A24" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A25" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A26" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A27" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A28" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A29" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A30" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A31" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A32" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="33" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A33" t="s">
         <v>40</v>
-      </c>
-    </row>
-    <row r="34" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A34" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="35" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A35" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="36" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A36" t="s">
-        <v>43</v>
       </c>
     </row>
   </sheetData>

</xml_diff>